<commit_message>
Updated for Visual Studio 2022
Updated test run for Visual Studio 2022, and updated the Excel
sheet with the latest test runs on Linux and Windows.
</commit_message>
<xml_diff>
--- a/Vectorsum_speed.xlsx
+++ b/Vectorsum_speed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\magnus\testspeed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus\src\testiteration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13506D5-13D3-4B0C-8AD1-4E5AADF19D28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A91924-7286-4CB0-A062-E3C9156D9AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="420" windowWidth="28065" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25200" yWindow="960" windowWidth="24705" windowHeight="21075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Comparison of summation of a vector of ints, 1E9 elements</t>
   </si>
@@ -96,13 +96,118 @@
     <t>Vector std::accumulate()</t>
   </si>
   <si>
-    <t>gcc 10.1</t>
-  </si>
-  <si>
-    <t>clang 10.0</t>
-  </si>
-  <si>
-    <t>Visual Studio 2019</t>
+    <t>Linux Fedora 35</t>
+  </si>
+  <si>
+    <t>Windows 10 Home</t>
+  </si>
+  <si>
+    <t>clang 13.0</t>
+  </si>
+  <si>
+    <t>gcc 11.2</t>
+  </si>
+  <si>
+    <t>Vector std::for_each()</t>
+  </si>
+  <si>
+    <t>10.0.19044.1387</t>
+  </si>
+  <si>
+    <t>Visual Studio 2022,  19.30.30706</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>32 GB RAM</t>
+  </si>
+  <si>
+    <t>6 cores, 12 threads</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i7-8700, 3.2 GHz</t>
+  </si>
+  <si>
+    <t>8th gen, Coffee Lake</t>
+  </si>
+  <si>
+    <t>MSVC options:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /Od</t>
+  </si>
+  <si>
+    <t>Disables optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /O1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /O2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /Ob3</t>
+  </si>
+  <si>
+    <t>Aggressive inlining</t>
+  </si>
+  <si>
+    <t>Creates small code</t>
+  </si>
+  <si>
+    <t>Creates fast code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /arch:avx2</t>
+  </si>
+  <si>
+    <t>Enables the use of Intel Advanced Vector Extensions 2 instructions.</t>
+  </si>
+  <si>
+    <t>GCC options</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Og</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -O1</t>
+  </si>
+  <si>
+    <t>Optimize</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -O2</t>
+  </si>
+  <si>
+    <t>Optimize even more, nearly all optimizations that do not involve a space-speed tradeoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -O3</t>
+  </si>
+  <si>
+    <t>Optimize yet more</t>
+  </si>
+  <si>
+    <t>Optimize debugging experience</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -march=haswell</t>
+  </si>
+  <si>
+    <t>Enable instructions found on Haswell and later CPUs</t>
+  </si>
+  <si>
+    <t>Clang options</t>
+  </si>
+  <si>
+    <t>Like -O1</t>
+  </si>
+  <si>
+    <t>Moderate level of optimization which enables most optimizations</t>
+  </si>
+  <si>
+    <t>Like -O2, except that it enables optimizations that take longer to perform or that may generate larger code (in an attempt to make the program run faster)</t>
   </si>
 </sst>
 </file>
@@ -432,15 +537,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H25"/>
+  <dimension ref="A2:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
@@ -448,14 +553,15 @@
     <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
@@ -477,410 +583,626 @@
       <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="C5" s="3">
-        <v>718</v>
+        <v>809</v>
       </c>
       <c r="D5" s="3">
-        <v>713</v>
+        <v>751</v>
       </c>
       <c r="E5" s="3">
-        <v>499</v>
+        <v>357</v>
       </c>
       <c r="F5" s="3">
-        <v>343</v>
+        <v>358</v>
       </c>
       <c r="G5" s="3">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="H5" s="3">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="C6" s="3">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="D6" s="3">
-        <v>412</v>
+        <v>505</v>
       </c>
       <c r="E6" s="3">
-        <v>343</v>
+        <v>498</v>
       </c>
       <c r="F6" s="3">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="G6" s="3">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="H6" s="3">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+      <c r="I6" s="3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="C7" s="3">
-        <v>348</v>
+        <v>363</v>
       </c>
       <c r="D7" s="3">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="E7" s="3">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="F7" s="3">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="G7" s="3">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="H7" s="3">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="I7" s="3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C8" s="3">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D8" s="3">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E8" s="3">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F8" s="3">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G8" s="3">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H8" s="3">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="I8" s="3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C9" s="3">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D9" s="3">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E9" s="3">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F9" s="3">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="G9" s="3">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H9" s="3">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="I9" s="3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>1853</v>
+        <v>351</v>
       </c>
       <c r="C10" s="3">
-        <v>4572</v>
+        <v>349</v>
       </c>
       <c r="D10" s="3">
-        <v>7775</v>
+        <v>351</v>
       </c>
       <c r="E10" s="3">
-        <v>4511</v>
+        <v>351</v>
       </c>
       <c r="F10" s="3">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="G10" s="3">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="H10" s="3">
-        <v>5475</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+      <c r="I10" s="3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <v>1860</v>
+        <v>349</v>
       </c>
       <c r="C11" s="3">
-        <v>4587</v>
+        <v>353</v>
       </c>
       <c r="D11" s="3">
-        <v>7754</v>
+        <v>351</v>
       </c>
       <c r="E11" s="3">
-        <v>4507</v>
+        <v>350</v>
       </c>
       <c r="F11" s="3">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="G11" s="3">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="H11" s="3">
-        <v>5474</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+      <c r="I11" s="3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C12" s="3">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D12" s="3">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E12" s="3">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F12" s="3">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="G12" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H12" s="3">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="I12" s="3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="3">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C13" s="3">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D13" s="3">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E13" s="3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F13" s="3">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G13" s="3">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="H13" s="3">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="I13" s="3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="3">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C14" s="3">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="D14" s="3">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E14" s="3">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F14" s="3">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G14" s="3">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="H14" s="3">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="I14" s="3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="3">
-        <v>3092</v>
+        <v>3009</v>
       </c>
       <c r="C15" s="3">
-        <v>3807</v>
+        <v>3760</v>
       </c>
       <c r="D15" s="3">
-        <v>4690</v>
+        <v>9025</v>
       </c>
       <c r="E15" s="3">
         <v>1643</v>
       </c>
       <c r="F15" s="3">
-        <v>1399</v>
+        <v>1401</v>
       </c>
       <c r="G15" s="3">
-        <v>1518</v>
+        <v>1521</v>
       </c>
       <c r="H15" s="3">
-        <v>2292</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2240</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="3">
-        <v>3093</v>
+        <v>286</v>
       </c>
       <c r="C16" s="3">
-        <v>3808</v>
+        <v>459</v>
       </c>
       <c r="D16" s="3">
-        <v>4699</v>
+        <v>478</v>
       </c>
       <c r="E16" s="3">
-        <v>1649</v>
+        <v>322</v>
       </c>
       <c r="F16" s="3">
-        <v>1400</v>
+        <v>315</v>
       </c>
       <c r="G16" s="3">
-        <v>1518</v>
+        <v>305</v>
       </c>
       <c r="H16" s="3">
-        <v>2294</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+      <c r="I16" s="3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="3">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="3">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D17" s="3">
-        <v>148</v>
+        <v>296</v>
       </c>
       <c r="E17" s="3">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F17" s="3">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G17" s="3">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H17" s="3">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="I17" s="3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="3">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C18" s="3">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D18" s="3">
-        <v>147</v>
+        <v>299</v>
       </c>
       <c r="E18" s="3">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F18" s="3">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G18" s="3">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="H18" s="3">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="I18" s="3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C19" s="3">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="D19" s="3">
+        <v>306</v>
+      </c>
+      <c r="E19" s="3">
+        <v>147</v>
+      </c>
+      <c r="F19" s="3">
+        <v>147</v>
+      </c>
+      <c r="G19" s="3">
         <v>157</v>
       </c>
-      <c r="E19" s="3">
-        <v>161</v>
-      </c>
-      <c r="F19" s="3">
-        <v>170</v>
-      </c>
-      <c r="G19" s="3">
-        <v>160</v>
-      </c>
       <c r="H19" s="3">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="I19" s="3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added BCC64, updated version of MSVC
Tests now also run using Embarcadero C++Builder bcc64, which is
based on clang/llvm.
Change option /Od for MSVC to /Os.
</commit_message>
<xml_diff>
--- a/Vectorsum_speed.xlsx
+++ b/Vectorsum_speed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus\src\testiteration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A91924-7286-4CB0-A062-E3C9156D9AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF3D6D0-1DDF-4D91-B909-754767EDF40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25200" yWindow="960" windowWidth="24705" windowHeight="21075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="135" windowWidth="23280" windowHeight="21075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
   <si>
     <t>Comparison of summation of a vector of ints, 1E9 elements</t>
   </si>
@@ -60,9 +60,6 @@
     <t>clang -O3 -march=haswell</t>
   </si>
   <si>
-    <t>msvc /Od</t>
-  </si>
-  <si>
     <t>msvc /O1</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Linux Fedora 35</t>
   </si>
   <si>
-    <t>Windows 10 Home</t>
-  </si>
-  <si>
     <t>clang 13.0</t>
   </si>
   <si>
@@ -111,12 +105,6 @@
     <t>Vector std::for_each()</t>
   </si>
   <si>
-    <t>10.0.19044.1387</t>
-  </si>
-  <si>
-    <t>Visual Studio 2022,  19.30.30706</t>
-  </si>
-  <si>
     <t>Hardware</t>
   </si>
   <si>
@@ -208,6 +196,42 @@
   </si>
   <si>
     <t>Like -O2, except that it enables optimizations that take longer to perform or that may generate larger code (in an attempt to make the program run faster)</t>
+  </si>
+  <si>
+    <t>bcc64 -Og</t>
+  </si>
+  <si>
+    <t>bcc64 -O1</t>
+  </si>
+  <si>
+    <t>bcc64 -O2</t>
+  </si>
+  <si>
+    <t>bcc64 -O3</t>
+  </si>
+  <si>
+    <t>bcc64 -O3 -march=haswell</t>
+  </si>
+  <si>
+    <t>msvc /Os</t>
+  </si>
+  <si>
+    <t>Windows 11 Home</t>
+  </si>
+  <si>
+    <t>10.0.22000.613</t>
+  </si>
+  <si>
+    <t>Visual Studio 2022,  19.31.31107</t>
+  </si>
+  <si>
+    <t>Embarcadero C++ 7.50 for Win64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bcc64 version 5.0.2 (d939c99b.1e953156.37585) (based on LLVM 5.0.2)</t>
+  </si>
+  <si>
+    <t>Embarcadero bcc64 options like Clang</t>
   </si>
 </sst>
 </file>
@@ -537,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I53"/>
+  <dimension ref="A2:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,28 +587,28 @@
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -879,298 +903,412 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3">
-        <v>3009</v>
+        <v>3268</v>
       </c>
       <c r="C15" s="3">
-        <v>3760</v>
+        <v>3915</v>
       </c>
       <c r="D15" s="3">
-        <v>9025</v>
+        <v>10708</v>
       </c>
       <c r="E15" s="3">
-        <v>1643</v>
+        <v>1704</v>
       </c>
       <c r="F15" s="3">
-        <v>1401</v>
+        <v>1482</v>
       </c>
       <c r="G15" s="3">
-        <v>1521</v>
+        <v>1598</v>
       </c>
       <c r="H15" s="3">
-        <v>2240</v>
+        <v>2854</v>
       </c>
       <c r="I15" s="3">
-        <v>1928</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>286</v>
+        <v>506</v>
       </c>
       <c r="C16" s="3">
-        <v>459</v>
+        <v>363</v>
       </c>
       <c r="D16" s="3">
-        <v>478</v>
+        <v>348</v>
       </c>
       <c r="E16" s="3">
-        <v>322</v>
+        <v>358</v>
       </c>
       <c r="F16" s="3">
-        <v>315</v>
+        <v>358</v>
       </c>
       <c r="G16" s="3">
-        <v>305</v>
+        <v>514</v>
       </c>
       <c r="H16" s="3">
-        <v>317</v>
+        <v>364</v>
       </c>
       <c r="I16" s="3">
-        <v>312</v>
+        <v>366</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="3">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="C17" s="3">
-        <v>308</v>
+        <v>365</v>
       </c>
       <c r="D17" s="3">
-        <v>296</v>
+        <v>349</v>
       </c>
       <c r="E17" s="3">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="F17" s="3">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="G17" s="3">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="H17" s="3">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="I17" s="3">
-        <v>303</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="3">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="C18" s="3">
-        <v>310</v>
+        <v>358</v>
       </c>
       <c r="D18" s="3">
-        <v>299</v>
+        <v>347</v>
       </c>
       <c r="E18" s="3">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="F18" s="3">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="G18" s="3">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="H18" s="3">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="I18" s="3">
-        <v>304</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C19" s="3">
-        <v>314</v>
+        <v>359</v>
       </c>
       <c r="D19" s="3">
-        <v>306</v>
+        <v>347</v>
       </c>
       <c r="E19" s="3">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F19" s="3">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G19" s="3">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H19" s="3">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I19" s="3">
-        <v>315</v>
-      </c>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3">
+        <v>9266</v>
+      </c>
+      <c r="C20" s="3">
+        <v>14486</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4739</v>
+      </c>
+      <c r="E20" s="3">
+        <v>6662</v>
+      </c>
+      <c r="F20" s="3">
+        <v>361</v>
+      </c>
+      <c r="G20" s="3">
+        <v>369</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1415</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="3">
+        <v>9234</v>
+      </c>
+      <c r="C21" s="3">
+        <v>14310</v>
+      </c>
+      <c r="D21" s="3">
+        <v>4724</v>
+      </c>
+      <c r="E21" s="3">
+        <v>6598</v>
+      </c>
+      <c r="F21" s="3">
+        <v>357</v>
+      </c>
+      <c r="G21" s="3">
+        <v>370</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1369</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="3">
+        <v>161</v>
+      </c>
+      <c r="C22" s="3">
+        <v>160</v>
+      </c>
+      <c r="D22" s="3">
+        <v>161</v>
+      </c>
+      <c r="E22" s="3">
+        <v>161</v>
+      </c>
+      <c r="F22" s="3">
+        <v>161</v>
+      </c>
+      <c r="G22" s="3">
+        <v>161</v>
+      </c>
+      <c r="H22" s="3">
+        <v>161</v>
+      </c>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B23" s="3">
+        <v>163</v>
+      </c>
+      <c r="C23" s="3">
+        <v>165</v>
+      </c>
+      <c r="D23" s="3">
+        <v>164</v>
+      </c>
+      <c r="E23" s="3">
+        <v>162</v>
+      </c>
+      <c r="F23" s="3">
+        <v>161</v>
+      </c>
+      <c r="G23" s="3">
+        <v>162</v>
+      </c>
+      <c r="H23" s="3">
+        <v>162</v>
+      </c>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="3">
+        <v>150</v>
+      </c>
+      <c r="C24" s="3">
+        <v>152</v>
+      </c>
+      <c r="D24" s="3">
+        <v>154</v>
+      </c>
+      <c r="E24" s="3">
+        <v>151</v>
+      </c>
+      <c r="F24" s="3">
+        <v>153</v>
+      </c>
+      <c r="G24" s="3">
+        <v>150</v>
+      </c>
+      <c r="H24" s="3">
+        <v>150</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="D25" t="s">
-        <v>28</v>
+      <c r="B28" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B43" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>44</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B48" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
         <v>47</v>
-      </c>
-      <c r="B49" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,26 +1321,60 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
         <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" t="s">
         <v>55</v>
       </c>
-      <c r="B53" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated optimization options in the Excel file
</commit_message>
<xml_diff>
--- a/Vectorsum_speed.xlsx
+++ b/Vectorsum_speed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus\src\testiteration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF3D6D0-1DDF-4D91-B909-754767EDF40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC559A9-1EC8-4C6A-8708-AE8FA6AD9414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6000" yWindow="135" windowWidth="23280" windowHeight="21075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,12 +66,6 @@
     <t>msvc /O2</t>
   </si>
   <si>
-    <t>msvc /O2 /Ob3</t>
-  </si>
-  <si>
-    <t>msvc /O2 /Ob3 /arch:avx2</t>
-  </si>
-  <si>
     <t>Vector [index]</t>
   </si>
   <si>
@@ -123,12 +117,6 @@
     <t>MSVC options:</t>
   </si>
   <si>
-    <t xml:space="preserve"> /Od</t>
-  </si>
-  <si>
-    <t>Disables optimization</t>
-  </si>
-  <si>
     <t xml:space="preserve"> /O1</t>
   </si>
   <si>
@@ -232,6 +220,18 @@
   </si>
   <si>
     <t>Embarcadero bcc64 options like Clang</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /Os</t>
+  </si>
+  <si>
+    <t>Optimze for space</t>
+  </si>
+  <si>
+    <t>msvc /O2 /Ob3 /favor:INTEL64</t>
+  </si>
+  <si>
+    <t>msvc /O2 /Ob3 /arch:avx2 /favor:INTEL64</t>
   </si>
 </sst>
 </file>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,28 +587,28 @@
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B15" s="3">
         <v>3268</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B18" s="3">
         <v>163</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="B19" s="3">
         <v>148</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B20" s="3">
         <v>9266</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B21" s="3">
         <v>9234</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="3">
         <v>161</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B23" s="3">
         <v>163</v>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B24" s="3">
         <v>150</v>
@@ -1183,198 +1183,198 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
         <v>28</v>
-      </c>
-      <c r="D35" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
         <v>34</v>
-      </c>
-      <c r="B41" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" t="s">
         <v>35</v>
-      </c>
-      <c r="B42" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel sheet for Fedora 36 and BCC std::for_each
</commit_message>
<xml_diff>
--- a/Vectorsum_speed.xlsx
+++ b/Vectorsum_speed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus\src\testiteration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC559A9-1EC8-4C6A-8708-AE8FA6AD9414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A33956F-D0CB-45FC-8DC4-A0CD49FCB6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="135" windowWidth="23280" windowHeight="21075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25890" yWindow="-45" windowWidth="23280" windowHeight="21075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -87,15 +87,6 @@
     <t>Vector std::accumulate()</t>
   </si>
   <si>
-    <t>Linux Fedora 35</t>
-  </si>
-  <si>
-    <t>clang 13.0</t>
-  </si>
-  <si>
-    <t>gcc 11.2</t>
-  </si>
-  <si>
     <t>Vector std::for_each()</t>
   </si>
   <si>
@@ -232,6 +223,15 @@
   </si>
   <si>
     <t>msvc /O2 /Ob3 /arch:avx2 /favor:INTEL64</t>
+  </si>
+  <si>
+    <t>gcc 12.1</t>
+  </si>
+  <si>
+    <t>clang 14.0</t>
+  </si>
+  <si>
+    <t>Linux Fedora 36</t>
   </si>
 </sst>
 </file>
@@ -254,12 +254,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -274,13 +286,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="63"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +624,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -616,28 +632,28 @@
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>533</v>
+        <v>511</v>
       </c>
       <c r="C5" s="3">
-        <v>809</v>
+        <v>1408</v>
       </c>
       <c r="D5" s="3">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="E5" s="3">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="F5" s="3">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="G5" s="3">
         <v>352</v>
       </c>
       <c r="H5" s="3">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="I5" s="3">
-        <v>1266</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -645,28 +661,28 @@
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C6" s="3">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D6" s="3">
-        <v>505</v>
+        <v>352</v>
       </c>
       <c r="E6" s="3">
-        <v>498</v>
+        <v>347</v>
       </c>
       <c r="F6" s="3">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G6" s="3">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H6" s="3">
-        <v>498</v>
+        <v>350</v>
       </c>
       <c r="I6" s="3">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -674,86 +690,86 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="C7" s="3">
+        <v>371</v>
+      </c>
+      <c r="D7" s="3">
         <v>363</v>
       </c>
-      <c r="D7" s="3">
-        <v>351</v>
-      </c>
       <c r="E7" s="3">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F7" s="3">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="G7" s="3">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="H7" s="3">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="I7" s="3">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3">
-        <v>168</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="5">
         <v>167</v>
       </c>
-      <c r="D8" s="3">
+      <c r="C8" s="5">
+        <v>167</v>
+      </c>
+      <c r="D8" s="5">
         <v>166</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
+        <v>166</v>
+      </c>
+      <c r="F8" s="5">
+        <v>166</v>
+      </c>
+      <c r="G8" s="5">
+        <v>166</v>
+      </c>
+      <c r="H8" s="5">
+        <v>167</v>
+      </c>
+      <c r="I8" s="5">
         <v>165</v>
       </c>
-      <c r="F8" s="3">
-        <v>167</v>
-      </c>
-      <c r="G8" s="3">
-        <v>166</v>
-      </c>
-      <c r="H8" s="3">
-        <v>165</v>
-      </c>
-      <c r="I8" s="3">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3">
-        <v>143</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B9" s="7">
+        <v>145</v>
+      </c>
+      <c r="C9" s="7">
+        <v>162</v>
+      </c>
+      <c r="D9" s="7">
         <v>146</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="7">
         <v>144</v>
       </c>
-      <c r="E9" s="3">
-        <v>145</v>
-      </c>
-      <c r="F9" s="3">
-        <v>144</v>
-      </c>
-      <c r="G9" s="3">
-        <v>144</v>
-      </c>
-      <c r="H9" s="3">
-        <v>143</v>
-      </c>
-      <c r="I9" s="3">
-        <v>145</v>
+      <c r="F9" s="7">
+        <v>146</v>
+      </c>
+      <c r="G9" s="7">
+        <v>151</v>
+      </c>
+      <c r="H9" s="7">
+        <v>150</v>
+      </c>
+      <c r="I9" s="7">
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -761,28 +777,28 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C10" s="3">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="D10" s="3">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="E10" s="3">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="F10" s="3">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="G10" s="3">
-        <v>350</v>
+        <v>379</v>
       </c>
       <c r="H10" s="3">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="I10" s="3">
-        <v>350</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -790,28 +806,28 @@
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <v>349</v>
+        <v>370</v>
       </c>
       <c r="C11" s="3">
+        <v>356</v>
+      </c>
+      <c r="D11" s="3">
+        <v>364</v>
+      </c>
+      <c r="E11" s="3">
+        <v>377</v>
+      </c>
+      <c r="F11" s="3">
+        <v>361</v>
+      </c>
+      <c r="G11" s="3">
         <v>353</v>
       </c>
-      <c r="D11" s="3">
-        <v>351</v>
-      </c>
-      <c r="E11" s="3">
-        <v>350</v>
-      </c>
-      <c r="F11" s="3">
-        <v>353</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
+        <v>360</v>
+      </c>
+      <c r="I11" s="3">
         <v>352</v>
-      </c>
-      <c r="H11" s="3">
-        <v>349</v>
-      </c>
-      <c r="I11" s="3">
-        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -822,112 +838,112 @@
         <v>159</v>
       </c>
       <c r="C12" s="3">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D12" s="3">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E12" s="3">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F12" s="3">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="G12" s="3">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="H12" s="3">
         <v>160</v>
       </c>
       <c r="I12" s="3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
+        <v>160</v>
+      </c>
+      <c r="C13" s="5">
+        <v>161</v>
+      </c>
+      <c r="D13" s="5">
+        <v>162</v>
+      </c>
+      <c r="E13" s="5">
         <v>159</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="F13" s="5">
+        <v>159</v>
+      </c>
+      <c r="G13" s="5">
         <v>160</v>
       </c>
-      <c r="C13" s="3">
-        <v>160</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="H13" s="5">
         <v>159</v>
       </c>
-      <c r="E13" s="3">
-        <v>160</v>
-      </c>
-      <c r="F13" s="3">
-        <v>159</v>
-      </c>
-      <c r="G13" s="3">
-        <v>160</v>
-      </c>
-      <c r="H13" s="3">
-        <v>159</v>
-      </c>
-      <c r="I13" s="3">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="I13" s="5">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3">
-        <v>147</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B14" s="7">
+        <v>142</v>
+      </c>
+      <c r="C14" s="7">
+        <v>146</v>
+      </c>
+      <c r="D14" s="7">
+        <v>146</v>
+      </c>
+      <c r="E14" s="7">
+        <v>145</v>
+      </c>
+      <c r="F14" s="7">
         <v>148</v>
       </c>
-      <c r="D14" s="3">
-        <v>147</v>
-      </c>
-      <c r="E14" s="3">
-        <v>146</v>
-      </c>
-      <c r="F14" s="3">
-        <v>147</v>
-      </c>
-      <c r="G14" s="3">
-        <v>147</v>
-      </c>
-      <c r="H14" s="3">
-        <v>147</v>
-      </c>
-      <c r="I14" s="3">
-        <v>147</v>
+      <c r="G14" s="7">
+        <v>143</v>
+      </c>
+      <c r="H14" s="7">
+        <v>158</v>
+      </c>
+      <c r="I14" s="7">
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B15" s="3">
-        <v>3268</v>
+        <v>3273</v>
       </c>
       <c r="C15" s="3">
-        <v>3915</v>
+        <v>3937</v>
       </c>
       <c r="D15" s="3">
-        <v>10708</v>
+        <v>10605</v>
       </c>
       <c r="E15" s="3">
-        <v>1704</v>
+        <v>1761</v>
       </c>
       <c r="F15" s="3">
-        <v>1482</v>
+        <v>1529</v>
       </c>
       <c r="G15" s="3">
-        <v>1598</v>
+        <v>1608</v>
       </c>
       <c r="H15" s="3">
-        <v>2854</v>
+        <v>3028</v>
       </c>
       <c r="I15" s="3">
-        <v>1980</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -935,446 +951,456 @@
         <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>506</v>
+        <v>522</v>
       </c>
       <c r="C16" s="3">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="D16" s="3">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="E16" s="3">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="F16" s="3">
-        <v>358</v>
+        <v>381</v>
       </c>
       <c r="G16" s="3">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="H16" s="3">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="I16" s="3">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="3">
-        <v>165</v>
-      </c>
-      <c r="C17" s="3">
-        <v>365</v>
-      </c>
-      <c r="D17" s="3">
-        <v>349</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="B17" s="5">
+        <v>172</v>
+      </c>
+      <c r="C17" s="5">
+        <v>371</v>
+      </c>
+      <c r="D17" s="5">
+        <v>356</v>
+      </c>
+      <c r="E17" s="5">
+        <v>171</v>
+      </c>
+      <c r="F17" s="5">
         <v>169</v>
       </c>
-      <c r="F17" s="3">
-        <v>164</v>
-      </c>
-      <c r="G17" s="3">
-        <v>164</v>
-      </c>
-      <c r="H17" s="3">
-        <v>168</v>
-      </c>
-      <c r="I17" s="3">
-        <v>364</v>
+      <c r="G17" s="5">
+        <v>171</v>
+      </c>
+      <c r="H17" s="5">
+        <v>171</v>
+      </c>
+      <c r="I17" s="5">
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B18" s="3">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C18" s="3">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="D18" s="3">
-        <v>347</v>
+        <v>368</v>
       </c>
       <c r="E18" s="3">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F18" s="3">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G18" s="3">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H18" s="3">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="I18" s="3">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="3">
-        <v>148</v>
-      </c>
-      <c r="C19" s="3">
-        <v>359</v>
-      </c>
-      <c r="D19" s="3">
-        <v>347</v>
-      </c>
-      <c r="E19" s="3">
-        <v>149</v>
-      </c>
-      <c r="F19" s="3">
-        <v>149</v>
-      </c>
-      <c r="G19" s="3">
-        <v>154</v>
-      </c>
-      <c r="H19" s="3">
-        <v>154</v>
-      </c>
-      <c r="I19" s="3">
-        <v>362</v>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="7">
+        <v>161</v>
+      </c>
+      <c r="C19" s="7">
+        <v>367</v>
+      </c>
+      <c r="D19" s="7">
+        <v>367</v>
+      </c>
+      <c r="E19" s="7">
+        <v>156</v>
+      </c>
+      <c r="F19" s="7">
+        <v>159</v>
+      </c>
+      <c r="G19" s="7">
+        <v>160</v>
+      </c>
+      <c r="H19" s="7">
+        <v>159</v>
+      </c>
+      <c r="I19" s="7">
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3">
-        <v>9266</v>
+        <v>9228</v>
       </c>
       <c r="C20" s="3">
-        <v>14486</v>
+        <v>14882</v>
       </c>
       <c r="D20" s="3">
-        <v>4739</v>
+        <v>4131</v>
       </c>
       <c r="E20" s="3">
-        <v>6662</v>
+        <v>6716</v>
       </c>
       <c r="F20" s="3">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G20" s="3">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="H20" s="3">
-        <v>1415</v>
-      </c>
-      <c r="I20" s="3"/>
+        <v>1381</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1253</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3">
-        <v>9234</v>
+        <v>9113</v>
       </c>
       <c r="C21" s="3">
-        <v>14310</v>
+        <v>14948</v>
       </c>
       <c r="D21" s="3">
-        <v>4724</v>
+        <v>4278</v>
       </c>
       <c r="E21" s="3">
-        <v>6598</v>
+        <v>6762</v>
       </c>
       <c r="F21" s="3">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G21" s="3">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="H21" s="3">
-        <v>1369</v>
-      </c>
-      <c r="I21" s="3"/>
+        <v>1385</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1256</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B22" s="3">
+        <v>163</v>
+      </c>
+      <c r="C22" s="3">
         <v>161</v>
       </c>
-      <c r="C22" s="3">
-        <v>160</v>
-      </c>
       <c r="D22" s="3">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E22" s="3">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F22" s="3">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="G22" s="3">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="H22" s="3">
         <v>161</v>
       </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="3">
-        <v>163</v>
-      </c>
-      <c r="C23" s="3">
-        <v>165</v>
-      </c>
-      <c r="D23" s="3">
+      <c r="I22" s="3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="5">
+        <v>171</v>
+      </c>
+      <c r="C23" s="5">
+        <v>161</v>
+      </c>
+      <c r="D23" s="5">
         <v>164</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="5">
+        <v>161</v>
+      </c>
+      <c r="F23" s="5">
+        <v>171</v>
+      </c>
+      <c r="G23" s="5">
+        <v>164</v>
+      </c>
+      <c r="H23" s="5">
+        <v>170</v>
+      </c>
+      <c r="I23" s="5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="7">
+        <v>151</v>
+      </c>
+      <c r="C24" s="7">
+        <v>150</v>
+      </c>
+      <c r="D24" s="7">
+        <v>158</v>
+      </c>
+      <c r="E24" s="7">
+        <v>166</v>
+      </c>
+      <c r="F24" s="7">
+        <v>155</v>
+      </c>
+      <c r="G24" s="7">
+        <v>155</v>
+      </c>
+      <c r="H24" s="7">
         <v>162</v>
       </c>
-      <c r="F23" s="3">
-        <v>161</v>
-      </c>
-      <c r="G23" s="3">
-        <v>162</v>
-      </c>
-      <c r="H23" s="3">
-        <v>162</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="3">
-        <v>150</v>
-      </c>
-      <c r="C24" s="3">
-        <v>152</v>
-      </c>
-      <c r="D24" s="3">
-        <v>154</v>
-      </c>
-      <c r="E24" s="3">
-        <v>151</v>
-      </c>
-      <c r="F24" s="3">
-        <v>153</v>
-      </c>
-      <c r="G24" s="3">
-        <v>150</v>
-      </c>
-      <c r="H24" s="3">
-        <v>150</v>
-      </c>
-      <c r="I24" s="3"/>
+      <c r="I24" s="7">
+        <v>164</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B54" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for MSVC 19.34 and Windows 11 22H2
</commit_message>
<xml_diff>
--- a/Vectorsum_speed.xlsx
+++ b/Vectorsum_speed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus\src\testiteration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A33956F-D0CB-45FC-8DC4-A0CD49FCB6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0DC24D-6786-41E3-84B6-71AAA7556EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25890" yWindow="-45" windowWidth="23280" windowHeight="21075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25410" yWindow="795" windowWidth="26895" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -198,12 +198,6 @@
     <t>Windows 11 Home</t>
   </si>
   <si>
-    <t>10.0.22000.613</t>
-  </si>
-  <si>
-    <t>Visual Studio 2022,  19.31.31107</t>
-  </si>
-  <si>
     <t>Embarcadero C++ 7.50 for Win64</t>
   </si>
   <si>
@@ -232,6 +226,12 @@
   </si>
   <si>
     <t>Linux Fedora 36</t>
+  </si>
+  <si>
+    <t>10.0.22621.963</t>
+  </si>
+  <si>
+    <t>Visual Studio 2022,  19.34.31937</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -922,28 +922,28 @@
         <v>55</v>
       </c>
       <c r="B15" s="3">
-        <v>3273</v>
+        <v>3298</v>
       </c>
       <c r="C15" s="3">
-        <v>3937</v>
+        <v>3988</v>
       </c>
       <c r="D15" s="3">
-        <v>10605</v>
+        <v>10945</v>
       </c>
       <c r="E15" s="3">
-        <v>1761</v>
+        <v>1738</v>
       </c>
       <c r="F15" s="3">
-        <v>1529</v>
+        <v>1502</v>
       </c>
       <c r="G15" s="3">
-        <v>1608</v>
+        <v>1611</v>
       </c>
       <c r="H15" s="3">
-        <v>3028</v>
+        <v>2626</v>
       </c>
       <c r="I15" s="3">
-        <v>2021</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -951,28 +951,28 @@
         <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>522</v>
+        <v>356</v>
       </c>
       <c r="C16" s="3">
-        <v>371</v>
+        <v>537</v>
       </c>
       <c r="D16" s="3">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="E16" s="3">
-        <v>367</v>
+        <v>565</v>
       </c>
       <c r="F16" s="3">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="G16" s="3">
-        <v>517</v>
+        <v>388</v>
       </c>
       <c r="H16" s="3">
-        <v>366</v>
+        <v>544</v>
       </c>
       <c r="I16" s="3">
-        <v>369</v>
+        <v>534</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -980,54 +980,54 @@
         <v>12</v>
       </c>
       <c r="B17" s="5">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C17" s="5">
+        <v>380</v>
+      </c>
+      <c r="D17" s="5">
         <v>371</v>
       </c>
-      <c r="D17" s="5">
-        <v>356</v>
-      </c>
       <c r="E17" s="5">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="F17" s="5">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="G17" s="5">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="H17" s="5">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="I17" s="5">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="3">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="C18" s="3">
-        <v>367</v>
+        <v>383</v>
       </c>
       <c r="D18" s="3">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="E18" s="3">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="F18" s="3">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="G18" s="3">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="H18" s="3">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="I18" s="3">
         <v>370</v>
@@ -1035,31 +1035,31 @@
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="7">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C19" s="7">
-        <v>367</v>
+        <v>382</v>
       </c>
       <c r="D19" s="7">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E19" s="7">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="F19" s="7">
         <v>159</v>
       </c>
       <c r="G19" s="7">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H19" s="7">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I19" s="7">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1067,28 +1067,28 @@
         <v>50</v>
       </c>
       <c r="B20" s="3">
-        <v>9228</v>
+        <v>9227</v>
       </c>
       <c r="C20" s="3">
-        <v>14882</v>
+        <v>15173</v>
       </c>
       <c r="D20" s="3">
-        <v>4131</v>
+        <v>4319</v>
       </c>
       <c r="E20" s="3">
-        <v>6716</v>
+        <v>6837</v>
       </c>
       <c r="F20" s="3">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="G20" s="3">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="H20" s="3">
-        <v>1381</v>
+        <v>1393</v>
       </c>
       <c r="I20" s="3">
-        <v>1253</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1096,28 +1096,28 @@
         <v>51</v>
       </c>
       <c r="B21" s="3">
-        <v>9113</v>
+        <v>9167</v>
       </c>
       <c r="C21" s="3">
-        <v>14948</v>
+        <v>15037</v>
       </c>
       <c r="D21" s="3">
-        <v>4278</v>
+        <v>4235</v>
       </c>
       <c r="E21" s="3">
-        <v>6762</v>
+        <v>6792</v>
       </c>
       <c r="F21" s="3">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="G21" s="3">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="H21" s="3">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="I21" s="3">
-        <v>1256</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1125,28 +1125,28 @@
         <v>52</v>
       </c>
       <c r="B22" s="3">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="C22" s="3">
-        <v>161</v>
+        <v>211</v>
       </c>
       <c r="D22" s="3">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E22" s="3">
+        <v>164</v>
+      </c>
+      <c r="F22" s="3">
         <v>166</v>
       </c>
-      <c r="F22" s="3">
-        <v>176</v>
-      </c>
       <c r="G22" s="3">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H22" s="3">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="I22" s="3">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1157,25 +1157,25 @@
         <v>171</v>
       </c>
       <c r="C23" s="5">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D23" s="5">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E23" s="5">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F23" s="5">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G23" s="5">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H23" s="5">
+        <v>184</v>
+      </c>
+      <c r="I23" s="5">
         <v>170</v>
-      </c>
-      <c r="I23" s="5">
-        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1183,63 +1183,63 @@
         <v>54</v>
       </c>
       <c r="B24" s="7">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C24" s="7">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D24" s="7">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E24" s="7">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F24" s="7">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G24" s="7">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="H24" s="7">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="I24" s="7">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
         <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,10 +1270,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test run with MSVC 19.42.34436
</commit_message>
<xml_diff>
--- a/Vectorsum_speed.xlsx
+++ b/Vectorsum_speed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus\src\testiteration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0DC24D-6786-41E3-84B6-71AAA7556EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCF9973-6F2E-486A-A81F-E2E876E7D1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25410" yWindow="795" windowWidth="26895" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18090" yWindow="480" windowWidth="28785" windowHeight="20610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -219,19 +219,19 @@
     <t>msvc /O2 /Ob3 /arch:avx2 /favor:INTEL64</t>
   </si>
   <si>
-    <t>gcc 12.1</t>
-  </si>
-  <si>
-    <t>clang 14.0</t>
-  </si>
-  <si>
-    <t>Linux Fedora 36</t>
-  </si>
-  <si>
-    <t>10.0.22621.963</t>
-  </si>
-  <si>
-    <t>Visual Studio 2022,  19.34.31937</t>
+    <t>10.0.22631.4751</t>
+  </si>
+  <si>
+    <t>Linux Fedora 41</t>
+  </si>
+  <si>
+    <t>gcc 14.2</t>
+  </si>
+  <si>
+    <t>clang 19.1</t>
+  </si>
+  <si>
+    <t>Visual Studio 2022,  19.42.34436</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A2:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,28 +632,28 @@
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C5" s="3">
-        <v>1408</v>
+        <v>1176</v>
       </c>
       <c r="D5" s="3">
-        <v>745</v>
+        <v>576</v>
       </c>
       <c r="E5" s="3">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F5" s="3">
         <v>349</v>
       </c>
       <c r="G5" s="3">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H5" s="3">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="I5" s="3">
-        <v>1258</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -664,25 +664,25 @@
         <v>350</v>
       </c>
       <c r="C6" s="3">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D6" s="3">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E6" s="3">
         <v>347</v>
       </c>
       <c r="F6" s="3">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="G6" s="3">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="H6" s="3">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="I6" s="3">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -690,28 +690,28 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="C7" s="3">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="D7" s="3">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="E7" s="3">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F7" s="3">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="G7" s="3">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="H7" s="3">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="I7" s="3">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -719,28 +719,28 @@
         <v>4</v>
       </c>
       <c r="B8" s="5">
+        <v>165</v>
+      </c>
+      <c r="C8" s="5">
+        <v>166</v>
+      </c>
+      <c r="D8" s="5">
         <v>167</v>
       </c>
-      <c r="C8" s="5">
+      <c r="E8" s="5">
+        <v>168</v>
+      </c>
+      <c r="F8" s="5">
+        <v>168</v>
+      </c>
+      <c r="G8" s="5">
         <v>167</v>
       </c>
-      <c r="D8" s="5">
+      <c r="H8" s="5">
         <v>166</v>
       </c>
-      <c r="E8" s="5">
+      <c r="I8" s="5">
         <v>166</v>
-      </c>
-      <c r="F8" s="5">
-        <v>166</v>
-      </c>
-      <c r="G8" s="5">
-        <v>166</v>
-      </c>
-      <c r="H8" s="5">
-        <v>167</v>
-      </c>
-      <c r="I8" s="5">
-        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -748,28 +748,28 @@
         <v>5</v>
       </c>
       <c r="B9" s="7">
+        <v>144</v>
+      </c>
+      <c r="C9" s="7">
+        <v>146</v>
+      </c>
+      <c r="D9" s="7">
         <v>145</v>
       </c>
-      <c r="C9" s="7">
-        <v>162</v>
-      </c>
-      <c r="D9" s="7">
-        <v>146</v>
-      </c>
       <c r="E9" s="7">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F9" s="7">
         <v>146</v>
       </c>
       <c r="G9" s="7">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H9" s="7">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I9" s="7">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -777,28 +777,28 @@
         <v>6</v>
       </c>
       <c r="B10" s="3">
+        <v>345</v>
+      </c>
+      <c r="C10" s="3">
+        <v>346</v>
+      </c>
+      <c r="D10" s="3">
+        <v>348</v>
+      </c>
+      <c r="E10" s="3">
         <v>347</v>
       </c>
-      <c r="C10" s="3">
-        <v>358</v>
-      </c>
-      <c r="D10" s="3">
-        <v>361</v>
-      </c>
-      <c r="E10" s="3">
-        <v>346</v>
-      </c>
       <c r="F10" s="3">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="G10" s="3">
-        <v>379</v>
+        <v>349</v>
       </c>
       <c r="H10" s="3">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="I10" s="3">
-        <v>360</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -806,28 +806,28 @@
         <v>7</v>
       </c>
       <c r="B11" s="3">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="C11" s="3">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="D11" s="3">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="E11" s="3">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="F11" s="3">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="G11" s="3">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H11" s="3">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="I11" s="3">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -835,28 +835,28 @@
         <v>8</v>
       </c>
       <c r="B12" s="3">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C12" s="3">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D12" s="3">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E12" s="3">
         <v>162</v>
       </c>
       <c r="F12" s="3">
+        <v>159</v>
+      </c>
+      <c r="G12" s="3">
+        <v>161</v>
+      </c>
+      <c r="H12" s="3">
         <v>162</v>
       </c>
-      <c r="G12" s="3">
-        <v>165</v>
-      </c>
-      <c r="H12" s="3">
-        <v>160</v>
-      </c>
       <c r="I12" s="3">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -867,25 +867,25 @@
         <v>160</v>
       </c>
       <c r="C13" s="5">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D13" s="5">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E13" s="5">
+        <v>160</v>
+      </c>
+      <c r="F13" s="5">
+        <v>160</v>
+      </c>
+      <c r="G13" s="5">
         <v>159</v>
-      </c>
-      <c r="F13" s="5">
-        <v>159</v>
-      </c>
-      <c r="G13" s="5">
-        <v>160</v>
       </c>
       <c r="H13" s="5">
         <v>159</v>
       </c>
       <c r="I13" s="5">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -893,28 +893,28 @@
         <v>10</v>
       </c>
       <c r="B14" s="7">
+        <v>144</v>
+      </c>
+      <c r="C14" s="7">
+        <v>143</v>
+      </c>
+      <c r="D14" s="7">
         <v>142</v>
       </c>
-      <c r="C14" s="7">
-        <v>146</v>
-      </c>
-      <c r="D14" s="7">
-        <v>146</v>
-      </c>
       <c r="E14" s="7">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F14" s="7">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G14" s="7">
         <v>143</v>
       </c>
       <c r="H14" s="7">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="I14" s="7">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -922,28 +922,28 @@
         <v>55</v>
       </c>
       <c r="B15" s="3">
-        <v>3298</v>
+        <v>3274</v>
       </c>
       <c r="C15" s="3">
-        <v>3988</v>
+        <v>3980</v>
       </c>
       <c r="D15" s="3">
-        <v>10945</v>
+        <v>16122</v>
       </c>
       <c r="E15" s="3">
-        <v>1738</v>
+        <v>1727</v>
       </c>
       <c r="F15" s="3">
-        <v>1502</v>
+        <v>1505</v>
       </c>
       <c r="G15" s="3">
-        <v>1611</v>
+        <v>1599</v>
       </c>
       <c r="H15" s="3">
-        <v>2626</v>
+        <v>1937</v>
       </c>
       <c r="I15" s="3">
-        <v>2065</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -951,28 +951,28 @@
         <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>356</v>
+        <v>532</v>
       </c>
       <c r="C16" s="3">
-        <v>537</v>
+        <v>374</v>
       </c>
       <c r="D16" s="3">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E16" s="3">
-        <v>565</v>
+        <v>390</v>
       </c>
       <c r="F16" s="3">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="G16" s="3">
-        <v>388</v>
+        <v>525</v>
       </c>
       <c r="H16" s="3">
-        <v>544</v>
+        <v>370</v>
       </c>
       <c r="I16" s="3">
-        <v>534</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -980,28 +980,28 @@
         <v>12</v>
       </c>
       <c r="B17" s="5">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C17" s="5">
-        <v>380</v>
+        <v>396</v>
       </c>
       <c r="D17" s="5">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="E17" s="5">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F17" s="5">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="G17" s="5">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="H17" s="5">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="I17" s="5">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1009,28 +1009,28 @@
         <v>62</v>
       </c>
       <c r="B18" s="3">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C18" s="3">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="D18" s="3">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="E18" s="3">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="F18" s="3">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="G18" s="3">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="H18" s="3">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="I18" s="3">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1038,28 +1038,28 @@
         <v>63</v>
       </c>
       <c r="B19" s="7">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C19" s="7">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D19" s="7">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="E19" s="7">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="F19" s="7">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="G19" s="7">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H19" s="7">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I19" s="7">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1067,28 +1067,28 @@
         <v>50</v>
       </c>
       <c r="B20" s="3">
-        <v>9227</v>
+        <v>9172</v>
       </c>
       <c r="C20" s="3">
-        <v>15173</v>
+        <v>15245</v>
       </c>
       <c r="D20" s="3">
-        <v>4319</v>
+        <v>4250</v>
       </c>
       <c r="E20" s="3">
-        <v>6837</v>
+        <v>6778</v>
       </c>
       <c r="F20" s="3">
-        <v>370</v>
+        <v>391</v>
       </c>
       <c r="G20" s="3">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="H20" s="3">
-        <v>1393</v>
+        <v>1389</v>
       </c>
       <c r="I20" s="3">
-        <v>1284</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1096,28 +1096,28 @@
         <v>51</v>
       </c>
       <c r="B21" s="3">
-        <v>9167</v>
+        <v>9053</v>
       </c>
       <c r="C21" s="3">
-        <v>15037</v>
+        <v>15079</v>
       </c>
       <c r="D21" s="3">
-        <v>4235</v>
+        <v>4338</v>
       </c>
       <c r="E21" s="3">
-        <v>6792</v>
+        <v>6903</v>
       </c>
       <c r="F21" s="3">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G21" s="3">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="H21" s="3">
-        <v>1382</v>
+        <v>1411</v>
       </c>
       <c r="I21" s="3">
-        <v>1340</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1125,28 +1125,28 @@
         <v>52</v>
       </c>
       <c r="B22" s="3">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C22" s="3">
-        <v>211</v>
+        <v>167</v>
       </c>
       <c r="D22" s="3">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E22" s="3">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F22" s="3">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G22" s="3">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="H22" s="3">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="I22" s="3">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1154,28 +1154,28 @@
         <v>53</v>
       </c>
       <c r="B23" s="5">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="5">
+        <v>179</v>
+      </c>
+      <c r="D23" s="5">
+        <v>172</v>
+      </c>
+      <c r="E23" s="5">
+        <v>167</v>
+      </c>
+      <c r="F23" s="5">
         <v>169</v>
       </c>
-      <c r="D23" s="5">
-        <v>170</v>
-      </c>
-      <c r="E23" s="5">
+      <c r="G23" s="5">
+        <v>167</v>
+      </c>
+      <c r="H23" s="5">
         <v>168</v>
       </c>
-      <c r="F23" s="5">
-        <v>170</v>
-      </c>
-      <c r="G23" s="5">
+      <c r="I23" s="5">
         <v>169</v>
-      </c>
-      <c r="H23" s="5">
-        <v>184</v>
-      </c>
-      <c r="I23" s="5">
-        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1183,44 +1183,44 @@
         <v>54</v>
       </c>
       <c r="B24" s="7">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C24" s="7">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D24" s="7">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E24" s="7">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F24" s="7">
+        <v>160</v>
+      </c>
+      <c r="G24" s="7">
+        <v>161</v>
+      </c>
+      <c r="H24" s="7">
         <v>157</v>
       </c>
-      <c r="G24" s="7">
-        <v>160</v>
-      </c>
-      <c r="H24" s="7">
-        <v>154</v>
-      </c>
       <c r="I24" s="7">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
         <v>65</v>
-      </c>
-      <c r="B29" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
         <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>